<commit_message>
implemented create Batch with valid data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_API_Hackathon_LMS_011026\Team2-BridgeBuilders\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08385DCF-ADE6-4A84-95C3-BAC7CC6AC034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD84C3A-5D00-4A8F-AFB1-D7885B3D51BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="234">
   <si>
     <t>Scenario</t>
   </si>
@@ -238,9 +238,6 @@
     <t>PA</t>
   </si>
   <si>
-    <t>CreateUserWithValidData</t>
-  </si>
-  <si>
     <t>EST</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
     <t>ManagingaconcurrencyinJavausingthreads</t>
   </si>
   <si>
-    <t>NinjaA1A0e2@gmail.com</t>
-  </si>
-  <si>
     <t>MicroservicesWithJavaupython</t>
   </si>
   <si>
@@ -439,9 +433,6 @@
     <t>Automation1141</t>
   </si>
   <si>
-    <t>AWS111112</t>
-  </si>
-  <si>
     <t>AWS222222</t>
   </si>
   <si>
@@ -493,9 +484,6 @@
     <t>CreateUserWithMandatoryFieldsValidData</t>
   </si>
   <si>
-    <t>+91 9876543211</t>
-  </si>
-  <si>
     <t>CreateUserWithExistingPhoneNumber</t>
   </si>
   <si>
@@ -508,14 +496,248 @@
     <t>R03</t>
   </si>
   <si>
-    <t>+91 1266612352</t>
+    <t>CreateUserWithInvaliduserFirstName</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLastName</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLocation</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserPhoneNumber</t>
+  </si>
+  <si>
+    <t>+91 123456789</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserRoleStatus</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserTimeZone</t>
+  </si>
+  <si>
+    <t>Act</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserVisaStatus</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLoginEmail</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvalidLoginstatus</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterloginstatus</t>
+  </si>
+  <si>
+    <t>#@!'</t>
+  </si>
+  <si>
+    <t>Us-Citizen</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLoginEmail</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserVisaStatus</t>
+  </si>
+  <si>
+    <t>^&amp;*(</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserTimeZone</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserRoleStatus</t>
+  </si>
+  <si>
+    <t>$%^&amp;</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInroleId</t>
+  </si>
+  <si>
+    <t>*&amp;^%</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserPhoneNumber</t>
+  </si>
+  <si>
+    <t>@#$</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserMiddleName</t>
+  </si>
+  <si>
+    <t>#$%^</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLocation</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLinkedinUrl</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLastName</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserFirstName</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterWithNumericloginStatus</t>
+  </si>
+  <si>
+    <t>+91 1266612353</t>
+  </si>
+  <si>
+    <t>CreateUserWithNoAuth</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>+91 1234567892</t>
+  </si>
+  <si>
+    <t>tester02</t>
+  </si>
+  <si>
+    <t>tester03</t>
+  </si>
+  <si>
+    <t>tester04</t>
+  </si>
+  <si>
+    <t>tester05</t>
+  </si>
+  <si>
+    <t>tester06</t>
+  </si>
+  <si>
+    <t>tester07</t>
+  </si>
+  <si>
+    <t>tester08</t>
+  </si>
+  <si>
+    <t>tester09</t>
+  </si>
+  <si>
+    <t>tester10</t>
+  </si>
+  <si>
+    <t>tester11</t>
+  </si>
+  <si>
+    <t>tester12</t>
+  </si>
+  <si>
+    <t>tester13</t>
+  </si>
+  <si>
+    <t>tester14</t>
+  </si>
+  <si>
+    <t>tester15</t>
+  </si>
+  <si>
+    <t>tester16</t>
+  </si>
+  <si>
+    <t>tester17</t>
+  </si>
+  <si>
+    <t>tester18</t>
+  </si>
+  <si>
+    <t>tester19</t>
+  </si>
+  <si>
+    <t>+91 9876543251</t>
+  </si>
+  <si>
+    <t>+91 1266612359</t>
+  </si>
+  <si>
+    <t>NinjaA1@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja2@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja3@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja4@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja5@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja6@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja7@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja8@gmail.com</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserFirstName</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserLastName</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserLoginEmail</t>
+  </si>
+  <si>
+    <t>'+91 1266612353</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserPhoneNumber</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR01</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR02</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR03</t>
+  </si>
+  <si>
+    <t>DA111112</t>
+  </si>
+  <si>
+    <t>+91 1266612354</t>
+  </si>
+  <si>
+    <t>NinjaA6@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +773,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -573,7 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,6 +818,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -913,10 +1144,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -961,7 +1192,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,10 +1245,10 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>231</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1026,7 +1257,7 @@
         <v>6</v>
       </c>
       <c r="F2">
-        <v>16713</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>201</v>
@@ -1043,7 +1274,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -1069,10 +1300,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
         <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>138</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -1098,7 +1329,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1113,7 +1344,7 @@
         <v>400</v>
       </c>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
@@ -1127,7 +1358,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1139,7 +1370,7 @@
         <v>400</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
@@ -1153,7 +1384,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1168,7 +1399,7 @@
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>37</v>
@@ -1194,7 +1425,7 @@
         <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
@@ -1273,7 +1504,7 @@
         <v>404</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -1368,7 +1599,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1397,7 +1628,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1449,7 +1680,7 @@
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1472,13 +1703,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -1499,10 +1730,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1519,10 +1750,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1539,13 +1770,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1566,15 +1797,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
@@ -1650,10 +1881,10 @@
     </row>
     <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -1662,7 +1893,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
@@ -1674,28 +1905,28 @@
         <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>159</v>
+        <v>232</v>
       </c>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
       </c>
       <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
         <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>71</v>
       </c>
       <c r="O2" t="s">
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>130</v>
+        <v>233</v>
       </c>
       <c r="Q2">
         <v>201</v>
@@ -1704,77 +1935,807 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q3">
+        <v>201</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
+        <v>66</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>149</v>
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K4" t="s">
         <v>154</v>
-      </c>
-      <c r="K4" t="s">
-        <v>108</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
         <v>6</v>
       </c>
+      <c r="P4" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="Q4">
         <v>201</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="R4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="K6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" t="s">
+        <v>148</v>
+      </c>
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q6">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K7" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>152</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>155</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H10" t="s">
+        <v>160</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F11" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" t="s">
+        <v>196</v>
+      </c>
+      <c r="H12" t="s">
+        <v>153</v>
+      </c>
+      <c r="L12" t="s">
+        <v>165</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" t="s">
+        <v>197</v>
+      </c>
+      <c r="H13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M13" t="s">
+        <v>166</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" t="s">
+        <v>226</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16" t="s">
+        <v>200</v>
+      </c>
+      <c r="H16" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" t="s">
+        <v>226</v>
+      </c>
+      <c r="O16" t="s">
+        <v>165</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
+      <c r="H17" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H18" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" t="s">
+        <v>203</v>
+      </c>
+      <c r="H19" t="s">
+        <v>153</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F20" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M20" t="s">
+        <v>176</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
+      <c r="H21" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="L21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F22" t="s">
+        <v>206</v>
+      </c>
+      <c r="H22" t="s">
+        <v>153</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K22" t="s">
+        <v>181</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" t="s">
+        <v>207</v>
+      </c>
+      <c r="H23" t="s">
+        <v>153</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" t="s">
+        <v>208</v>
+      </c>
+      <c r="H24" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" t="s">
+        <v>185</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" t="s">
+        <v>209</v>
+      </c>
+      <c r="H25" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N25" t="s">
+        <v>185</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H26" t="s">
+        <v>179</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" t="s">
+        <v>179</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" t="s">
+        <v>181</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" t="s">
+        <v>185</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>190</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="O30">
+        <v>2345</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>223</v>
+      </c>
+      <c r="H31" t="s">
+        <v>146</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>224</v>
+      </c>
+      <c r="E32" t="s">
+        <v>212</v>
+      </c>
+      <c r="H32" t="s">
+        <v>146</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>225</v>
+      </c>
+      <c r="E33" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" t="s">
+        <v>210</v>
+      </c>
+      <c r="H33" t="s">
+        <v>146</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="E34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" t="s">
+        <v>212</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>192</v>
+      </c>
+      <c r="E35" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" t="s">
+        <v>146</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" t="s">
+        <v>149</v>
+      </c>
+      <c r="L35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M35" t="s">
         <v>147</v>
       </c>
-      <c r="F5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" t="s">
-        <v>158</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="N35" t="s">
+        <v>70</v>
+      </c>
+      <c r="O35" t="s">
         <v>6</v>
       </c>
-      <c r="M5" t="s">
-        <v>156</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" t="s">
+        <v>153</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L36" t="s">
         <v>6</v>
       </c>
-      <c r="Q5">
-        <v>400</v>
+      <c r="M36" t="s">
+        <v>147</v>
+      </c>
+      <c r="N36" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" t="s">
+        <v>6</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q36">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{955CB5D7-B530-42D7-97E8-42D9187F14F1}"/>
-    <hyperlink ref="P2" r:id="rId2" xr:uid="{B078AAA0-04BA-49BA-875C-2A6717595E25}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{955CB5D7-B530-42D7-97E8-42D9187F14F1}"/>
+    <hyperlink ref="P4" r:id="rId2" xr:uid="{B078AAA0-04BA-49BA-875C-2A6717595E25}"/>
+    <hyperlink ref="O17" r:id="rId3" xr:uid="{A4C0B0C2-5A15-4F46-A1A7-1C0BB8CF3318}"/>
+    <hyperlink ref="P6" r:id="rId4" xr:uid="{4C308BA6-2660-4F3E-BB02-553377917B3A}"/>
+    <hyperlink ref="P7" r:id="rId5" xr:uid="{079F20F4-DA21-424E-B459-28C91E9A482C}"/>
+    <hyperlink ref="P8" r:id="rId6" xr:uid="{107160F3-BF1C-4B8B-B9C7-DF19A7C0A2F6}"/>
+    <hyperlink ref="P9" r:id="rId7" xr:uid="{A84FB387-C4D1-4AA4-B3DC-B456F008929F}"/>
+    <hyperlink ref="P10" r:id="rId8" xr:uid="{CE98B7EB-7AEC-443E-8213-82693C1E7C30}"/>
+    <hyperlink ref="P11" r:id="rId9" xr:uid="{CA2200A2-08E7-44A5-8311-50C5FC03CE59}"/>
+    <hyperlink ref="P12" r:id="rId10" xr:uid="{85072F2F-8739-4F4D-8458-363C6C97F5B8}"/>
+    <hyperlink ref="P13" r:id="rId11" xr:uid="{EC5EB13A-C1C4-422B-B025-25DCDF114BC1}"/>
+    <hyperlink ref="P14:P16" r:id="rId12" display="Ninja8@gmail.com" xr:uid="{99F1AE56-81E5-4066-BD7F-F27FE5BFB914}"/>
+    <hyperlink ref="P17" r:id="rId13" xr:uid="{F0A66DC2-2112-4A8A-8B2E-650E24E3CDD3}"/>
+    <hyperlink ref="P21" r:id="rId14" xr:uid="{7F9731B2-6950-422A-8E4A-DE8AB6CF992F}"/>
+    <hyperlink ref="P25" r:id="rId15" xr:uid="{1D5386F4-24F2-404C-A34D-1B1D68E49616}"/>
+    <hyperlink ref="P29" r:id="rId16" xr:uid="{250E8EB2-D743-4BF9-BEFB-7BA4BE8ADEE2}"/>
+    <hyperlink ref="P34" r:id="rId17" xr:uid="{8F96F680-BCD3-4D73-ACB2-3258878A7FBB}"/>
+    <hyperlink ref="P18:P20" r:id="rId18" display="Ninja8@gmail.com" xr:uid="{E5AF81C8-A3F0-4DE4-9530-0591158A3C71}"/>
+    <hyperlink ref="P22:P24" r:id="rId19" display="Ninja8@gmail.com" xr:uid="{C4185873-227C-4A1C-9BFA-017C88EB208B}"/>
+    <hyperlink ref="P26:P28" r:id="rId20" display="Ninja8@gmail.com" xr:uid="{23347D6D-2376-45C6-A38C-7BD19A18D7B6}"/>
+    <hyperlink ref="P35:P36" r:id="rId21" display="Ninja8@gmail.com" xr:uid="{6CEBBF05-0DDB-47CD-9328-A29CEFEF45BB}"/>
+    <hyperlink ref="G2" r:id="rId22" xr:uid="{73B57736-9737-4E56-8EF7-3AD2C6E42FCB}"/>
+    <hyperlink ref="P2" r:id="rId23" xr:uid="{FA1A68E9-2B2D-4A4F-B42C-1840DD121756}"/>
+    <hyperlink ref="G3" r:id="rId24" xr:uid="{EBF33BE8-7319-4ACD-8BB7-12E8E9E68B21}"/>
+    <hyperlink ref="P3" r:id="rId25" xr:uid="{86B298D4-95FA-4FA4-9C65-ED6ED5191C26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1805,25 +2766,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -1834,35 +2795,35 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="4">
         <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1871,23 +2832,23 @@
         <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1896,45 +2857,45 @@
         <v>400</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="4">
         <v>400</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1943,35 +2904,35 @@
         <v>400</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="4">
         <v>400</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1981,13 +2942,13 @@
         <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1997,16 +2958,16 @@
         <v>200</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2016,51 +2977,51 @@
         <v>200</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="6">
         <v>200</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -2069,38 +3030,38 @@
         <v>200</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="4">
         <v>200</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2110,13 +3071,13 @@
         <v>200</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2126,38 +3087,38 @@
         <v>200</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="4">
         <v>201</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>

</xml_diff>

<commit_message>
Created Separated classes to build POJO for user and batch module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_API_Hackathon_LMS_011026\Team2-BridgeBuilders\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD84C3A-5D00-4A8F-AFB1-D7885B3D51BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0A2BCA-0432-40F7-9309-DA8AAE0651B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="236">
   <si>
     <t>Scenario</t>
   </si>
@@ -724,13 +724,19 @@
     <t>CreateUserWithValidDataR03</t>
   </si>
   <si>
-    <t>DA111112</t>
-  </si>
-  <si>
-    <t>+91 1266612354</t>
-  </si>
-  <si>
-    <t>NinjaA6@gmail.com</t>
+    <t>CreateBatchWithValidDataFP</t>
+  </si>
+  <si>
+    <t>UnitTesting11</t>
+  </si>
+  <si>
+    <t>Python11112</t>
+  </si>
+  <si>
+    <t>NinjaA34@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 1666698881</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,82 +1214,56 @@
     <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D2">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>201</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>232</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3">
-        <v>16713</v>
+        <v>39</v>
       </c>
       <c r="G3">
         <v>201</v>
@@ -1291,28 +1271,25 @@
       <c r="I3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4">
-        <v>16713</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>201</v>
@@ -1326,25 +1303,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G5">
-        <v>400</v>
-      </c>
-      <c r="H5" t="s">
-        <v>110</v>
+        <v>201</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
@@ -1355,22 +1329,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6">
         <v>16713</v>
       </c>
       <c r="G6">
-        <v>400</v>
-      </c>
-      <c r="H6" t="s">
-        <v>111</v>
+        <v>201</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
@@ -1381,25 +1358,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>37</v>
@@ -1410,12 +1387,12 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
       </c>
       <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8">
@@ -1425,7 +1402,7 @@
         <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
@@ -1436,17 +1413,26 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
       <c r="F9">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G9">
         <v>400</v>
       </c>
+      <c r="H9" t="s">
+        <v>112</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1456,16 +1442,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -1474,37 +1454,33 @@
         <v>16713</v>
       </c>
       <c r="G10">
-        <v>401</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="H10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -1512,51 +1488,55 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G12">
-        <v>400</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="I12" s="1"/>
       <c r="J12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13">
-        <v>16653</v>
+        <v>16713</v>
       </c>
       <c r="G13">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
         <v>15</v>
@@ -1564,22 +1544,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>400</v>
@@ -1593,45 +1567,45 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15">
-        <v>16713</v>
+        <v>16653</v>
       </c>
       <c r="G15">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -1640,30 +1614,36 @@
         <v>16713</v>
       </c>
       <c r="G16">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G17">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>37</v>
@@ -1674,16 +1654,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -1692,7 +1672,7 @@
         <v>16713</v>
       </c>
       <c r="G18">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>37</v>
@@ -1703,37 +1683,39 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>401</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1742,7 +1724,10 @@
         <v>16713</v>
       </c>
       <c r="G20">
-        <v>200</v>
+        <v>400</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1750,10 +1735,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1762,21 +1753,19 @@
         <v>16713</v>
       </c>
       <c r="G21">
-        <v>400</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="I21" s="1"/>
       <c r="J21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1785,6 +1774,49 @@
         <v>16713</v>
       </c>
       <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>16713</v>
+      </c>
+      <c r="G23">
+        <v>400</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>16713</v>
+      </c>
+      <c r="G24">
         <v>404</v>
       </c>
     </row>
@@ -1800,7 +1832,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1908,7 +1940,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K2" t="s">
         <v>149</v>
@@ -1926,7 +1958,7 @@
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Q2">
         <v>201</v>

</xml_diff>

<commit_message>
program get modules added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1D93A40F-35C3-40E7-8447-4C8CAF6BA67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5BB7ECAA-2EDC-4D87-8087-A51FA50CE351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,11 +11,11 @@
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Batch" sheetId="1" r:id="rId2"/>
     <sheet name="User" sheetId="3" r:id="rId3"/>
-    <sheet name="program" sheetId="5" r:id="rId4"/>
+    <sheet name="Program" sheetId="5" r:id="rId4"/>
     <sheet name="skill" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E5"/>
+  <oleSize ref="B1:F8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>Scenario</t>
   </si>
@@ -261,30 +261,9 @@
     <t>Automation124</t>
   </si>
   <si>
-    <t>Bad Request</t>
-  </si>
-  <si>
-    <t>InActive</t>
-  </si>
-  <si>
-    <t>rewrw</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>scenario</t>
-  </si>
-  <si>
     <t>ExpectedContentType</t>
   </si>
   <si>
-    <t>Expected StatusMessage</t>
-  </si>
-  <si>
-    <t>Expected Statuscode</t>
-  </si>
-  <si>
     <t>ProgramStatus</t>
   </si>
   <si>
@@ -414,18 +393,6 @@
     <t>Valid request body</t>
   </si>
   <si>
-    <t>RestAssuredlearning</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>NewProgram</t>
-  </si>
-  <si>
-    <t>Fitness</t>
-  </si>
-  <si>
     <t>Invalid request body</t>
   </si>
   <si>
@@ -436,6 +403,15 @@
   </si>
   <si>
     <t>Basics</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>iuoiughbkh</t>
+  </si>
+  <si>
+    <t>jbhvdxcfjhbm</t>
   </si>
 </sst>
 </file>
@@ -840,10 +816,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -941,10 +917,10 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -970,7 +946,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -996,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -1025,7 +1001,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1040,7 +1016,7 @@
         <v>400</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
@@ -1054,7 +1030,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1066,7 +1042,7 @@
         <v>400</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
@@ -1080,7 +1056,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1095,7 +1071,7 @@
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>37</v>
@@ -1121,7 +1097,7 @@
         <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
@@ -1295,7 +1271,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1324,7 +1300,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1405,7 +1381,7 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -1426,10 +1402,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1446,10 +1422,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1466,13 +1442,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
         <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1495,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1589,7 +1565,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
@@ -1604,10 +1580,10 @@
         <v>73</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -1622,7 +1598,7 @@
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q2">
         <v>201</v>
@@ -1633,31 +1609,31 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="N4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="O4" t="s">
         <v>6</v>
@@ -1668,28 +1644,28 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="L5" t="s">
         <v>6</v>
       </c>
       <c r="M5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="O5" t="s">
         <v>6</v>
@@ -1712,7 +1688,7 @@
   <dimension ref="A1:K190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1722,52 +1698,45 @@
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="27.90625" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="37.08984375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="26.6328125" customWidth="1"/>
-    <col min="10" max="10" width="16.6328125" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="6" max="6" width="37.08984375" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="26.6328125" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
         <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1775,737 +1744,662 @@
       <c r="E2" s="4">
         <v>201</v>
       </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
+      <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>132</v>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="E3" s="4">
-        <v>201</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="E4" s="4">
         <v>400</v>
       </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="4">
-        <v>400</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="4"/>
+      <c r="F5" s="1"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E6" s="4"/>
-      <c r="G6" s="1"/>
+    </row>
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D7" s="4"/>
-      <c r="F7" s="1"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D8" s="4"/>
-      <c r="F8" s="1"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D9" s="4"/>
-      <c r="F9" s="1"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D10" s="4"/>
-      <c r="F10" s="1"/>
+    </row>
+    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+    </row>
+    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="4"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="1"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="1"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="1"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="1"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="1"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D16" s="4"/>
-      <c r="F16" s="1"/>
+    </row>
+    <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="4"/>
+      <c r="E16" s="1"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C17" s="4"/>
-      <c r="E17" s="1"/>
+    </row>
+    <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D18" s="4"/>
-      <c r="F18" s="1"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="3:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="4"/>
-      <c r="F19" s="1"/>
+    </row>
+    <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="1"/>
+    </row>
+    <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D21" s="4"/>
-      <c r="F21" s="1"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D22" s="4"/>
-      <c r="F22" s="1"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D23" s="4"/>
-      <c r="F23" s="1"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D24" s="4"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D26" s="4"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D27" s="4"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="4"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="4"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D36" s="4"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D37" s="4"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D162" s="4"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D163" s="4"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D164" s="4"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D165" s="4"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D166" s="4"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D168" s="4"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D169" s="4"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D170" s="4"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D171" s="4"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D172" s="4"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D173" s="4"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D174" s="4"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D176" s="4"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D183" s="4"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D184" s="4"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D187" s="4"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D188" s="4"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D190" s="4"/>
-    </row>
+    <row r="190" spans="1:11" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{D87B51C5-D291-4CA8-85C5-B9DA3EE47FFB}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{D87B51C5-D291-4CA8-85C5-B9DA3EE47FFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Retrieved program id, batch id for chaining
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_API_Hackathon_LMS_011026\Team2-BridgeBuilders\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0A2BCA-0432-40F7-9309-DA8AAE0651B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAC67A0-C585-4360-B6B2-D2DE8E92BC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Batch" sheetId="1" r:id="rId2"/>
     <sheet name="User" sheetId="3" r:id="rId3"/>
-    <sheet name="program" sheetId="5" r:id="rId4"/>
-    <sheet name="skill" sheetId="6" r:id="rId5"/>
+    <sheet name="Program" sheetId="5" r:id="rId4"/>
+    <sheet name="Skill" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="242">
   <si>
     <t>Scenario</t>
   </si>
@@ -334,18 +334,12 @@
     <t>valid ( POST)</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
     <t>ExpectedContentType</t>
   </si>
   <si>
     <t>Expected StatusMessage</t>
   </si>
   <si>
-    <t>Expected Statuscode</t>
-  </si>
-  <si>
     <t>ProgramStatus</t>
   </si>
   <si>
@@ -391,9 +385,6 @@
     <t>ProgramDescription</t>
   </si>
   <si>
-    <t>WebautomationusingSeleniumWebDriver</t>
-  </si>
-  <si>
     <t>BasicsofJavaincludingsyntaxandOOP</t>
   </si>
   <si>
@@ -733,10 +724,37 @@
     <t>Python11112</t>
   </si>
   <si>
-    <t>NinjaA34@gmail.com</t>
-  </si>
-  <si>
-    <t>+91 1666698881</t>
+    <t>Valid request bodyFB</t>
+  </si>
+  <si>
+    <t>Valid request bodyFDPID</t>
+  </si>
+  <si>
+    <t>Valid request bodyFDPN</t>
+  </si>
+  <si>
+    <t>qqqqqqqqqqq</t>
+  </si>
+  <si>
+    <t>cccc</t>
+  </si>
+  <si>
+    <t>WebautomationusingSele</t>
+  </si>
+  <si>
+    <t>AWSprgg</t>
+  </si>
+  <si>
+    <t>azureprgg</t>
+  </si>
+  <si>
+    <t>Cloudprgg</t>
+  </si>
+  <si>
+    <t>+91 1666618881</t>
+  </si>
+  <si>
+    <t>NinjaA35@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1168,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -1198,7 +1216,7 @@
   <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1248,13 +1266,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1277,10 +1295,10 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1306,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1332,10 +1350,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1361,7 +1379,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1376,7 +1394,7 @@
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>37</v>
@@ -1390,7 +1408,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1402,7 +1420,7 @@
         <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
@@ -1416,7 +1434,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1431,7 +1449,7 @@
         <v>400</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>37</v>
@@ -1457,7 +1475,7 @@
         <v>400</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>37</v>
@@ -1631,7 +1649,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D17">
         <v>14</v>
@@ -1660,7 +1678,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D18">
         <v>15</v>
@@ -1741,7 +1759,7 @@
         <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -1762,10 +1780,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1782,10 +1800,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
@@ -1802,13 +1820,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
         <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -1831,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1913,7 +1931,7 @@
     </row>
     <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>
@@ -1925,7 +1943,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
@@ -1940,10 +1958,10 @@
         <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="K2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -1958,7 +1976,7 @@
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="Q2">
         <v>201</v>
@@ -1969,7 +1987,7 @@
     </row>
     <row r="3" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
         <v>71</v>
@@ -1981,7 +1999,7 @@
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
         <v>66</v>
@@ -1996,10 +2014,10 @@
         <v>72</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -2014,7 +2032,7 @@
         <v>6</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q3">
         <v>201</v>
@@ -2025,7 +2043,7 @@
     </row>
     <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
         <v>71</v>
@@ -2037,7 +2055,7 @@
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -2052,10 +2070,10 @@
         <v>72</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
@@ -2070,7 +2088,7 @@
         <v>6</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q4">
         <v>201</v>
@@ -2081,37 +2099,37 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
         <v>144</v>
       </c>
-      <c r="F6" t="s">
+      <c r="N6" t="s">
         <v>145</v>
       </c>
-      <c r="H6" t="s">
-        <v>146</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="K6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" t="s">
-        <v>147</v>
-      </c>
-      <c r="N6" t="s">
-        <v>148</v>
-      </c>
-      <c r="O6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="Q6">
         <v>201</v>
@@ -2119,34 +2137,34 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" t="s">
         <v>151</v>
       </c>
-      <c r="E7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" t="s">
-        <v>153</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K7" t="s">
-        <v>154</v>
-      </c>
       <c r="L7" t="s">
         <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="O7" t="s">
         <v>6</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="Q7">
         <v>400</v>
@@ -2154,130 +2172,130 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q14">
         <v>400</v>
@@ -2285,412 +2303,412 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F22" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F23" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F26" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E27" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
+        <v>178</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F28" t="s">
-        <v>181</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="P28" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O30">
         <v>2345</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E32" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E33" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K35" t="s">
+        <v>146</v>
+      </c>
+      <c r="L35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M35" t="s">
         <v>144</v>
-      </c>
-      <c r="F35" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" t="s">
-        <v>146</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="K35" t="s">
-        <v>149</v>
-      </c>
-      <c r="L35" t="s">
-        <v>6</v>
-      </c>
-      <c r="M35" t="s">
-        <v>147</v>
       </c>
       <c r="N35" t="s">
         <v>70</v>
@@ -2699,7 +2717,7 @@
         <v>6</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q35">
         <v>401</v>
@@ -2707,25 +2725,25 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="L36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" t="s">
         <v>144</v>
-      </c>
-      <c r="F36" t="s">
-        <v>144</v>
-      </c>
-      <c r="H36" t="s">
-        <v>153</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L36" t="s">
-        <v>6</v>
-      </c>
-      <c r="M36" t="s">
-        <v>147</v>
       </c>
       <c r="N36" t="s">
         <v>70</v>
@@ -2734,7 +2752,7 @@
         <v>6</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q36">
         <v>404</v>
@@ -2775,10 +2793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE89BC8E-AB0C-48F9-875D-2818F98F0AD7}">
-  <dimension ref="A1:K190"/>
+  <dimension ref="A1:K192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2798,25 +2816,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -2827,13 +2845,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4">
         <v>201</v>
@@ -2845,17 +2863,17 @@
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>231</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>131</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2864,70 +2882,73 @@
         <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>232</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>239</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4">
-        <v>400</v>
+        <v>201</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>233</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
+        <v>118</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
-        <v>400</v>
+        <v>201</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -2942,18 +2963,21 @@
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>124</v>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>92</v>
       </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
       <c r="D7" s="4">
         <v>400</v>
       </c>
@@ -2964,42 +2988,51 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
       <c r="D9" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -3015,32 +3048,23 @@
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>200</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" t="s">
         <v>78</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
         <v>85</v>
@@ -3049,41 +3073,32 @@
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
       <c r="D12" s="4">
         <v>200</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" t="s">
         <v>78</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="4">
+        <v>126</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="6">
         <v>200</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -3093,12 +3108,24 @@
         <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
       <c r="D14" s="4">
         <v>200</v>
       </c>
@@ -3109,12 +3136,21 @@
         <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
       <c r="D15" s="4">
         <v>200</v>
       </c>
@@ -3125,115 +3161,138 @@
         <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" t="s">
-        <v>82</v>
-      </c>
       <c r="D16" s="4">
-        <v>201</v>
-      </c>
-      <c r="E16" t="s">
-        <v>99</v>
+        <v>200</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C17" s="4"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D17" s="4">
+        <v>200</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D18" s="4"/>
-      <c r="F18" s="1"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="4">
+        <v>201</v>
+      </c>
+      <c r="E18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>100</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="3:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="4"/>
-      <c r="F19" s="1"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C19" s="4"/>
+      <c r="E19" s="1"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D20" s="4"/>
       <c r="F20" s="1"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D21" s="4"/>
       <c r="F21" s="1"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D22" s="4"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="1"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D23" s="4"/>
       <c r="F23" s="1"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D24" s="4"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D26" s="4"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
       <c r="F32" s="1"/>
@@ -3244,11 +3303,11 @@
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.35">
@@ -3257,13 +3316,16 @@
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D38" s="4"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D39" s="4"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D40" s="4"/>
@@ -3717,6 +3779,12 @@
     </row>
     <row r="190" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D190" s="4"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D191" s="4"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D192" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Assigned User to Program and batch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\RestAssured_API_Hackathon_LMS_011026\Team2-BridgeBuilders\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAC67A0-C585-4360-B6B2-D2DE8E92BC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1338A02A-40DE-4B06-BDE8-73A85F0DFA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="258">
   <si>
     <t>Scenario</t>
   </si>
@@ -661,15 +661,6 @@
     <t>tester19</t>
   </si>
   <si>
-    <t>+91 9876543251</t>
-  </si>
-  <si>
-    <t>+91 1266612359</t>
-  </si>
-  <si>
-    <t>NinjaA1@gmail.com</t>
-  </si>
-  <si>
     <t>Ninja2@gmail.com</t>
   </si>
   <si>
@@ -742,19 +733,76 @@
     <t>WebautomationusingSele</t>
   </si>
   <si>
-    <t>AWSprgg</t>
-  </si>
-  <si>
-    <t>azureprgg</t>
-  </si>
-  <si>
-    <t>Cloudprgg</t>
-  </si>
-  <si>
-    <t>+91 1666618881</t>
-  </si>
-  <si>
-    <t>NinjaA35@gmail.com</t>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatchStatus</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithValidData</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithInvalidAdminId</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithMissingMandatoryField</t>
+  </si>
+  <si>
+    <t>U123</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>U34</t>
+  </si>
+  <si>
+    <t>+91 1267612359</t>
+  </si>
+  <si>
+    <t>+91 9876643251</t>
+  </si>
+  <si>
+    <t>"+91 9876643251</t>
+  </si>
+  <si>
+    <t>NinjaAC1@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 3266612359</t>
+  </si>
+  <si>
+    <t>NinjaAB2@gmail.com</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithValidAdminId</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithInvalidAdminId</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithMissingMandatoryField</t>
+  </si>
+  <si>
+    <t>AWSf</t>
+  </si>
+  <si>
+    <t>azuref</t>
+  </si>
+  <si>
+    <t>Cloudf</t>
+  </si>
+  <si>
+    <t>+91 8265778881</t>
+  </si>
+  <si>
+    <t>NinjaA48@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1266,13 +1314,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
         <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1298,7 +1346,7 @@
         <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1847,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1871,9 +1919,11 @@
     <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1928,10 +1978,22 @@
       <c r="R1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="S1" t="s">
+        <v>234</v>
+      </c>
+      <c r="T1" t="s">
+        <v>236</v>
+      </c>
+      <c r="U1" t="s">
+        <v>235</v>
+      </c>
+      <c r="V1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>
@@ -1958,7 +2020,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="K2" t="s">
         <v>146</v>
@@ -1976,7 +2038,7 @@
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="Q2">
         <v>201</v>
@@ -1985,9 +2047,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
         <v>71</v>
@@ -2014,7 +2076,7 @@
         <v>72</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="K3" t="s">
         <v>105</v>
@@ -2032,7 +2094,7 @@
         <v>6</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>212</v>
+        <v>249</v>
       </c>
       <c r="Q3">
         <v>201</v>
@@ -2041,9 +2103,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
         <v>71</v>
@@ -2070,7 +2132,7 @@
         <v>72</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>211</v>
+        <v>244</v>
       </c>
       <c r="K4" t="s">
         <v>151</v>
@@ -2088,7 +2150,7 @@
         <v>6</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="Q4">
         <v>201</v>
@@ -2097,7 +2159,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -2111,7 +2173,7 @@
         <v>143</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="K6" t="s">
         <v>105</v>
@@ -2129,13 +2191,13 @@
         <v>6</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="Q6">
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2149,7 +2211,7 @@
         <v>150</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>188</v>
+        <v>246</v>
       </c>
       <c r="K7" t="s">
         <v>151</v>
@@ -2164,13 +2226,13 @@
         <v>6</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Q7">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -2178,10 +2240,13 @@
         <v>153</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+      <c r="Q8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -2192,10 +2257,13 @@
         <v>155</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+      <c r="Q9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -2209,10 +2277,13 @@
         <v>157</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+      <c r="Q10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2229,10 +2300,13 @@
         <v>159</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="Q11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>160</v>
       </c>
@@ -2249,10 +2323,13 @@
         <v>162</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>161</v>
       </c>
@@ -2272,10 +2349,13 @@
         <v>163</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -2289,19 +2369,19 @@
         <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N14" t="s">
         <v>165</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="Q14">
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -2315,13 +2395,16 @@
         <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q15">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>167</v>
       </c>
@@ -2335,16 +2418,19 @@
         <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O16" t="s">
         <v>162</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -2364,10 +2450,13 @@
         <v>169</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -2384,10 +2473,13 @@
         <v>188</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -2407,10 +2499,13 @@
         <v>170</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -2430,10 +2525,13 @@
         <v>173</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -2453,10 +2551,13 @@
         <v>176</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q21">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>177</v>
       </c>
@@ -2476,10 +2577,13 @@
         <v>178</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>179</v>
       </c>
@@ -2496,10 +2600,13 @@
         <v>180</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q23">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2519,10 +2626,13 @@
         <v>188</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -2542,10 +2652,13 @@
         <v>182</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>183</v>
       </c>
@@ -2562,10 +2675,13 @@
         <v>188</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>184</v>
       </c>
@@ -2579,10 +2695,13 @@
         <v>188</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q27">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>185</v>
       </c>
@@ -2593,10 +2712,13 @@
         <v>188</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q28">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>186</v>
       </c>
@@ -2607,10 +2729,13 @@
         <v>188</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -2621,12 +2746,15 @@
         <v>2345</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H31" t="s">
         <v>143</v>
@@ -2635,10 +2763,13 @@
         <v>188</v>
       </c>
       <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E32" t="s">
         <v>209</v>
@@ -2650,12 +2781,15 @@
         <v>188</v>
       </c>
       <c r="P32" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q32">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>222</v>
       </c>
       <c r="E33" t="s">
         <v>209</v>
@@ -2670,10 +2804,13 @@
         <v>188</v>
       </c>
       <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q33">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
         <v>209</v>
@@ -2682,10 +2819,13 @@
         <v>209</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+      <c r="Q34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -2717,13 +2857,13 @@
         <v>6</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="Q35">
         <v>401</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -2752,10 +2892,88 @@
         <v>6</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="Q36">
         <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>238</v>
+      </c>
+      <c r="K40" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q40">
+        <v>200</v>
+      </c>
+      <c r="S40" t="s">
+        <v>241</v>
+      </c>
+      <c r="V40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q41">
+        <v>404</v>
+      </c>
+      <c r="S41" t="s">
+        <v>243</v>
+      </c>
+      <c r="V41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q42">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>250</v>
+      </c>
+      <c r="K45" t="s">
+        <v>146</v>
+      </c>
+      <c r="L45" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>251</v>
+      </c>
+      <c r="K46" t="s">
+        <v>105</v>
+      </c>
+      <c r="L46" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q46">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q47">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -2845,10 +3063,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -2863,17 +3081,17 @@
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2888,17 +3106,17 @@
         <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -2913,7 +3131,7 @@
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>

</xml_diff>

<commit_message>
update and delete request
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2A43B3DC-A858-4BF1-9F0C-AC65CE54986B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\preet\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17809FD9-F4E7-47EE-B6EB-626DF287C37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,10 +17,9 @@
     <sheet name="Batch" sheetId="1" r:id="rId2"/>
     <sheet name="User" sheetId="3" r:id="rId3"/>
     <sheet name="Program" sheetId="5" r:id="rId4"/>
-    <sheet name="skill" sheetId="6" r:id="rId5"/>
+    <sheet name="Skill" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="B1:E4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="249">
   <si>
     <t>Scenario</t>
   </si>
@@ -234,9 +238,6 @@
     <t>PA</t>
   </si>
   <si>
-    <t>CreateUserWithValidData</t>
-  </si>
-  <si>
     <t>EST</t>
   </si>
   <si>
@@ -261,9 +262,33 @@
     <t>Automation124</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>APIA</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
     <t>ExpectedContentType</t>
   </si>
   <si>
+    <t>Expected StatusMessage</t>
+  </si>
+  <si>
+    <t>ProgramStatus</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
     <t>R02</t>
   </si>
   <si>
@@ -300,7 +325,13 @@
     <t>UpdateBatchWithInvalidBatchId</t>
   </si>
   <si>
-    <t>NinjaA1A0e2@gmail.com</t>
+    <t>ProgramDescription</t>
+  </si>
+  <si>
+    <t>LearningApirestassure</t>
+  </si>
+  <si>
+    <t>JavaReflectionTest</t>
   </si>
   <si>
     <t>Automation11221</t>
@@ -309,9 +340,6 @@
     <t>Automation1141</t>
   </si>
   <si>
-    <t>AWS111112</t>
-  </si>
-  <si>
     <t>AWS222222</t>
   </si>
   <si>
@@ -363,9 +391,6 @@
     <t>CreateUserWithMandatoryFieldsValidData</t>
   </si>
   <si>
-    <t>+91 9876543211</t>
-  </si>
-  <si>
     <t>CreateUserWithExistingPhoneNumber</t>
   </si>
   <si>
@@ -378,53 +403,386 @@
     <t>R03</t>
   </si>
   <si>
-    <t>+91 1266612352</t>
-  </si>
-  <si>
-    <t>Valid request body</t>
-  </si>
-  <si>
-    <t>Invalid request body</t>
-  </si>
-  <si>
-    <t>#@$()</t>
+    <t>CreateUserWithInvaliduserFirstName</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLastName</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLocation</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserPhoneNumber</t>
+  </si>
+  <si>
+    <t>+91 123456789</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserRoleStatus</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserTimeZone</t>
+  </si>
+  <si>
+    <t>Act</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserVisaStatus</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvaliduserLoginEmail</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvalidLoginstatus</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterloginstatus</t>
+  </si>
+  <si>
+    <t>#@!'</t>
+  </si>
+  <si>
+    <t>Us-Citizen</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLoginEmail</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserVisaStatus</t>
+  </si>
+  <si>
+    <t>^&amp;*(</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserTimeZone</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserRoleStatus</t>
+  </si>
+  <si>
+    <t>$%^&amp;</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInroleId</t>
+  </si>
+  <si>
+    <t>*&amp;^%</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserPhoneNumber</t>
+  </si>
+  <si>
+    <t>@#$</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserMiddleName</t>
+  </si>
+  <si>
+    <t>#$%^</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLocation</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLinkedinUrl</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserLastName</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterInuserFirstName</t>
+  </si>
+  <si>
+    <t>CreateUserWithSpecialCharacterWithNumericloginStatus</t>
+  </si>
+  <si>
+    <t>+91 1266612353</t>
+  </si>
+  <si>
+    <t>CreateUserWithNoAuth</t>
+  </si>
+  <si>
+    <t>CreateUserWithInvalidEndpoint</t>
+  </si>
+  <si>
+    <t>+91 1234567892</t>
+  </si>
+  <si>
+    <t>tester02</t>
+  </si>
+  <si>
+    <t>tester03</t>
+  </si>
+  <si>
+    <t>tester04</t>
+  </si>
+  <si>
+    <t>tester05</t>
+  </si>
+  <si>
+    <t>tester06</t>
+  </si>
+  <si>
+    <t>tester07</t>
+  </si>
+  <si>
+    <t>tester08</t>
+  </si>
+  <si>
+    <t>tester09</t>
+  </si>
+  <si>
+    <t>tester10</t>
+  </si>
+  <si>
+    <t>tester11</t>
+  </si>
+  <si>
+    <t>tester12</t>
+  </si>
+  <si>
+    <t>tester13</t>
+  </si>
+  <si>
+    <t>tester14</t>
+  </si>
+  <si>
+    <t>tester15</t>
+  </si>
+  <si>
+    <t>tester16</t>
+  </si>
+  <si>
+    <t>tester17</t>
+  </si>
+  <si>
+    <t>tester18</t>
+  </si>
+  <si>
+    <t>tester19</t>
+  </si>
+  <si>
+    <t>Ninja2@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja3@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja4@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja5@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja6@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja7@gmail.com</t>
+  </si>
+  <si>
+    <t>Ninja8@gmail.com</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserFirstName</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserLastName</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserLoginEmail</t>
+  </si>
+  <si>
+    <t>'+91 1266612353</t>
+  </si>
+  <si>
+    <t>CreateUserWithEmptyuserPhoneNumber</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR01</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR02</t>
+  </si>
+  <si>
+    <t>CreateUserWithValidDataR03</t>
+  </si>
+  <si>
+    <t>Python11112</t>
+  </si>
+  <si>
+    <t>Valid request bodyFB</t>
+  </si>
+  <si>
+    <t>Valid request bodyFDPID</t>
+  </si>
+  <si>
+    <t>Valid request bodyFDPN</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>batchId</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatchStatus</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithValidData</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithInvalidAdminId</t>
+  </si>
+  <si>
+    <t>AssignAdminToProgramBatchWithMissingMandatoryField</t>
+  </si>
+  <si>
+    <t>U123</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>U34</t>
+  </si>
+  <si>
+    <t>+91 9876643251</t>
+  </si>
+  <si>
+    <t>"+91 9876643251</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithValidAdminId</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithInvalidAdminId</t>
+  </si>
+  <si>
+    <t>UpdateAdminRoleStatusWithMissingMandatoryField</t>
+  </si>
+  <si>
+    <t>+91 9265778881</t>
+  </si>
+  <si>
+    <t>NinjaA49@gmail.com</t>
+  </si>
+  <si>
+    <t>UpdateAdminWithValidAdminIdAndValidData</t>
+  </si>
+  <si>
+    <t>UpdateAdminWithInvalidAdminIdAndValidData</t>
+  </si>
+  <si>
+    <t>UpdateAdminWithMissingMandatoryFields</t>
+  </si>
+  <si>
+    <t>+91 9446161140</t>
+  </si>
+  <si>
+    <t>+91 3266612340</t>
+  </si>
+  <si>
+    <t>+91 1267612340</t>
+  </si>
+  <si>
+    <t>NinjaA536@gmail.com</t>
+  </si>
+  <si>
+    <t>NinjaAB3@gmail.com</t>
+  </si>
+  <si>
+    <t>NinjaAC2@gmail.com</t>
+  </si>
+  <si>
+    <t>welcomenewworld</t>
+  </si>
+  <si>
+    <t>welcomeall</t>
+  </si>
+  <si>
+    <t>welcomenewworld1</t>
+  </si>
+  <si>
+    <t>welcomenewworld2</t>
+  </si>
+  <si>
+    <t>welcomeall1</t>
+  </si>
+  <si>
+    <t>welcomeall2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid request body	</t>
   </si>
   <si>
     <t>Missing request body</t>
   </si>
   <si>
-    <t>Basics</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>programDescription</t>
-  </si>
-  <si>
-    <t>programName</t>
-  </si>
-  <si>
-    <t>programStatus</t>
-  </si>
-  <si>
-    <t>jkhvuhjmw2</t>
-  </si>
-  <si>
-    <t>APIREstA12</t>
-  </si>
-  <si>
-    <t>dfbst12</t>
-  </si>
-  <si>
-    <t>iygkijbhia2</t>
+    <t>%YW$%</t>
+  </si>
+  <si>
+    <t>ValidMandatoryField</t>
+  </si>
+  <si>
+    <t>MissingMandatoryField</t>
+  </si>
+  <si>
+    <t>InvalidMandatoryField</t>
+  </si>
+  <si>
+    <t>iamhap</t>
+  </si>
+  <si>
+    <t>afdhsdghP</t>
+  </si>
+  <si>
+    <t>ValidRequest</t>
+  </si>
+  <si>
+    <t>MissingRequest</t>
+  </si>
+  <si>
+    <t>InvalidRequest</t>
+  </si>
+  <si>
+    <t>APIAasgkhbssaqi</t>
+  </si>
+  <si>
+    <t>Helloworld</t>
+  </si>
+  <si>
+    <t>dgnhmty</t>
+  </si>
+  <si>
+    <t>vxdvdfb</t>
+  </si>
+  <si>
+    <t>$%&amp;$(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +818,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -482,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -500,9 +864,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -825,10 +1190,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -870,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A2:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,111 +1254,59 @@
     <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>16713</v>
-      </c>
-      <c r="G2">
-        <v>201</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>16713</v>
-      </c>
-      <c r="G3">
-        <v>201</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>197</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4">
-        <v>16713</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>201</v>
@@ -1007,25 +1320,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G5">
-        <v>400</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
+        <v>201</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
@@ -1036,22 +1346,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6">
         <v>16713</v>
       </c>
       <c r="G6">
-        <v>400</v>
-      </c>
-      <c r="H6" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
@@ -1062,25 +1375,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7" t="s">
         <v>89</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>16713</v>
-      </c>
-      <c r="G7">
-        <v>400</v>
-      </c>
-      <c r="H7" t="s">
-        <v>84</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>37</v>
@@ -1091,12 +1404,12 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
       </c>
       <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8">
@@ -1106,7 +1419,7 @@
         <v>400</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>37</v>
@@ -1117,16 +1430,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
       <c r="F9">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G9">
         <v>400</v>
+      </c>
+      <c r="H9" t="s">
+        <v>91</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>37</v>
@@ -1137,16 +1459,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -1155,37 +1471,33 @@
         <v>16713</v>
       </c>
       <c r="G10">
-        <v>401</v>
-      </c>
-      <c r="I10" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -1193,51 +1505,55 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G12">
-        <v>400</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="I12" s="1"/>
       <c r="J12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13">
-        <v>16653</v>
+        <v>16713</v>
       </c>
       <c r="G13">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
         <v>15</v>
@@ -1245,22 +1561,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>400</v>
@@ -1274,45 +1584,45 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15">
-        <v>16713</v>
+        <v>16653</v>
       </c>
       <c r="G15">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -1321,30 +1631,36 @@
         <v>16713</v>
       </c>
       <c r="G16">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>16713</v>
       </c>
       <c r="G17">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>37</v>
@@ -1355,16 +1671,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
@@ -1373,7 +1689,7 @@
         <v>16713</v>
       </c>
       <c r="G18">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>37</v>
@@ -1384,37 +1700,39 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>16713</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>401</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1423,7 +1741,10 @@
         <v>16713</v>
       </c>
       <c r="G20">
-        <v>200</v>
+        <v>400</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1431,10 +1752,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>107</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1443,21 +1770,19 @@
         <v>16713</v>
       </c>
       <c r="G21">
-        <v>400</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="I21" s="1"/>
       <c r="J21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1466,6 +1791,49 @@
         <v>16713</v>
       </c>
       <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>16713</v>
+      </c>
+      <c r="G23">
+        <v>400</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>16713</v>
+      </c>
+      <c r="G24">
         <v>404</v>
       </c>
     </row>
@@ -1478,15 +1846,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0883ED9D-FC09-4A47-93CF-B3A51E2E4694}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
@@ -1502,9 +1870,11 @@
     <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1559,13 +1929,25 @@
       <c r="R1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="S1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T1" t="s">
+        <v>203</v>
+      </c>
+      <c r="U1" t="s">
+        <v>202</v>
+      </c>
+      <c r="V1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -1574,7 +1956,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
@@ -1586,28 +1968,28 @@
         <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>117</v>
+        <v>221</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
       </c>
       <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
         <v>70</v>
       </c>
-      <c r="N2" t="s">
-        <v>71</v>
-      </c>
       <c r="O2" t="s">
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>91</v>
+        <v>224</v>
       </c>
       <c r="Q2">
         <v>201</v>
@@ -1616,77 +1998,1131 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="K3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q3">
+        <v>201</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>66</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>112</v>
+        <v>223</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="L4" t="s">
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
         <v>6</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="Q4">
         <v>201</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="R4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" t="s">
         <v>113</v>
       </c>
-      <c r="E5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J6" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" t="s">
         <v>117</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q6">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+      <c r="H12" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" t="s">
+        <v>134</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M13" t="s">
+        <v>135</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+      <c r="H14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" t="s">
+        <v>192</v>
+      </c>
+      <c r="N14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" t="s">
+        <v>122</v>
+      </c>
+      <c r="J15" t="s">
+        <v>192</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q15">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" t="s">
+        <v>192</v>
+      </c>
+      <c r="O16" t="s">
+        <v>134</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H20" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M20" t="s">
+        <v>145</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L21" t="s">
+        <v>148</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q21">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F23" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" t="s">
+        <v>122</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q23">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" t="s">
+        <v>177</v>
+      </c>
+      <c r="H24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" t="s">
+        <v>154</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N25" t="s">
+        <v>154</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" t="s">
+        <v>179</v>
+      </c>
+      <c r="H26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" t="s">
+        <v>181</v>
+      </c>
+      <c r="G27" t="s">
+        <v>148</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q27">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q28">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O30">
+        <v>2345</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H31" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="E32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q32">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" t="s">
+        <v>181</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+      <c r="H35" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K35" t="s">
+        <v>118</v>
+      </c>
+      <c r="L35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M35" t="s">
         <v>116</v>
       </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" t="s">
-        <v>114</v>
-      </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q5">
-        <v>400</v>
+      <c r="N35" t="s">
+        <v>70</v>
+      </c>
+      <c r="O35" t="s">
+        <v>6</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" t="s">
+        <v>116</v>
+      </c>
+      <c r="N36" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" t="s">
+        <v>6</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q36">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>205</v>
+      </c>
+      <c r="K40" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q40">
+        <v>200</v>
+      </c>
+      <c r="S40" t="s">
+        <v>208</v>
+      </c>
+      <c r="V40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+      <c r="K41" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q41">
+        <v>404</v>
+      </c>
+      <c r="S41" t="s">
+        <v>210</v>
+      </c>
+      <c r="V41" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q42">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>213</v>
+      </c>
+      <c r="K45" t="s">
+        <v>118</v>
+      </c>
+      <c r="L45" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>214</v>
+      </c>
+      <c r="K46" t="s">
+        <v>86</v>
+      </c>
+      <c r="L46" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q46">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q47">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" t="s">
+        <v>72</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K50" t="s">
+        <v>118</v>
+      </c>
+      <c r="L50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M50" t="s">
+        <v>69</v>
+      </c>
+      <c r="N50" t="s">
+        <v>70</v>
+      </c>
+      <c r="O50" t="s">
+        <v>6</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q50">
+        <v>201</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>219</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H51" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" t="s">
+        <v>72</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+      <c r="L51" t="s">
+        <v>6</v>
+      </c>
+      <c r="M51" t="s">
+        <v>69</v>
+      </c>
+      <c r="N51" t="s">
+        <v>70</v>
+      </c>
+      <c r="O51" t="s">
+        <v>6</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q51">
+        <v>404</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I52" t="s">
+        <v>72</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K52" t="s">
+        <v>118</v>
+      </c>
+      <c r="L52" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" t="s">
+        <v>69</v>
+      </c>
+      <c r="N52" t="s">
+        <v>70</v>
+      </c>
+      <c r="O52" t="s">
+        <v>6</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q52">
+        <v>400</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{955CB5D7-B530-42D7-97E8-42D9187F14F1}"/>
-    <hyperlink ref="P2" r:id="rId2" xr:uid="{B078AAA0-04BA-49BA-875C-2A6717595E25}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{955CB5D7-B530-42D7-97E8-42D9187F14F1}"/>
+    <hyperlink ref="P4" r:id="rId2" xr:uid="{B078AAA0-04BA-49BA-875C-2A6717595E25}"/>
+    <hyperlink ref="O17" r:id="rId3" xr:uid="{A4C0B0C2-5A15-4F46-A1A7-1C0BB8CF3318}"/>
+    <hyperlink ref="P6" r:id="rId4" xr:uid="{4C308BA6-2660-4F3E-BB02-553377917B3A}"/>
+    <hyperlink ref="P7" r:id="rId5" xr:uid="{079F20F4-DA21-424E-B459-28C91E9A482C}"/>
+    <hyperlink ref="P8" r:id="rId6" xr:uid="{107160F3-BF1C-4B8B-B9C7-DF19A7C0A2F6}"/>
+    <hyperlink ref="P9" r:id="rId7" xr:uid="{A84FB387-C4D1-4AA4-B3DC-B456F008929F}"/>
+    <hyperlink ref="P10" r:id="rId8" xr:uid="{CE98B7EB-7AEC-443E-8213-82693C1E7C30}"/>
+    <hyperlink ref="P11" r:id="rId9" xr:uid="{CA2200A2-08E7-44A5-8311-50C5FC03CE59}"/>
+    <hyperlink ref="P12" r:id="rId10" xr:uid="{85072F2F-8739-4F4D-8458-363C6C97F5B8}"/>
+    <hyperlink ref="P13" r:id="rId11" xr:uid="{EC5EB13A-C1C4-422B-B025-25DCDF114BC1}"/>
+    <hyperlink ref="P14:P16" r:id="rId12" display="Ninja8@gmail.com" xr:uid="{99F1AE56-81E5-4066-BD7F-F27FE5BFB914}"/>
+    <hyperlink ref="P17" r:id="rId13" xr:uid="{F0A66DC2-2112-4A8A-8B2E-650E24E3CDD3}"/>
+    <hyperlink ref="P21" r:id="rId14" xr:uid="{7F9731B2-6950-422A-8E4A-DE8AB6CF992F}"/>
+    <hyperlink ref="P25" r:id="rId15" xr:uid="{1D5386F4-24F2-404C-A34D-1B1D68E49616}"/>
+    <hyperlink ref="P29" r:id="rId16" xr:uid="{250E8EB2-D743-4BF9-BEFB-7BA4BE8ADEE2}"/>
+    <hyperlink ref="P34" r:id="rId17" xr:uid="{8F96F680-BCD3-4D73-ACB2-3258878A7FBB}"/>
+    <hyperlink ref="P18:P20" r:id="rId18" display="Ninja8@gmail.com" xr:uid="{E5AF81C8-A3F0-4DE4-9530-0591158A3C71}"/>
+    <hyperlink ref="P22:P24" r:id="rId19" display="Ninja8@gmail.com" xr:uid="{C4185873-227C-4A1C-9BFA-017C88EB208B}"/>
+    <hyperlink ref="P26:P28" r:id="rId20" display="Ninja8@gmail.com" xr:uid="{23347D6D-2376-45C6-A38C-7BD19A18D7B6}"/>
+    <hyperlink ref="P35:P36" r:id="rId21" display="Ninja8@gmail.com" xr:uid="{6CEBBF05-0DDB-47CD-9328-A29CEFEF45BB}"/>
+    <hyperlink ref="G2" r:id="rId22" xr:uid="{73B57736-9737-4E56-8EF7-3AD2C6E42FCB}"/>
+    <hyperlink ref="P2" r:id="rId23" xr:uid="{FA1A68E9-2B2D-4A4F-B42C-1840DD121756}"/>
+    <hyperlink ref="G3" r:id="rId24" xr:uid="{EBF33BE8-7319-4ACD-8BB7-12E8E9E68B21}"/>
+    <hyperlink ref="P3" r:id="rId25" xr:uid="{86B298D4-95FA-4FA4-9C65-ED6ED5191C26}"/>
+    <hyperlink ref="G50" r:id="rId26" xr:uid="{AF7924AD-7AAC-4459-B5A0-CE7FF108FA37}"/>
+    <hyperlink ref="P50" r:id="rId27" xr:uid="{C4396201-3978-49A8-9910-79A22E2C1B03}"/>
+    <hyperlink ref="G51" r:id="rId28" xr:uid="{C9A1DE0C-6728-45A9-B6EE-FA2049AA1E3E}"/>
+    <hyperlink ref="P51" r:id="rId29" xr:uid="{4F7C61DB-3964-4868-B6C0-C2E88031EF04}"/>
+    <hyperlink ref="G52" r:id="rId30" xr:uid="{15DB91B5-5982-4455-B9FB-A33E987873A5}"/>
+    <hyperlink ref="P52" r:id="rId31" xr:uid="{B1D062A8-337B-4FBB-B75E-27200562F2F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1694,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE89BC8E-AB0C-48F9-875D-2818F98F0AD7}">
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1707,732 +3143,908 @@
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="27.90625" customWidth="1"/>
-    <col min="6" max="6" width="37.08984375" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="37.08984375" customWidth="1"/>
     <col min="8" max="8" width="26.6328125" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="9">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4">
         <v>201</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>118</v>
+      <c r="G2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
         <v>201</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="G3" t="s">
+        <v>199</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4">
-        <v>400</v>
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>201</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="G4" t="s">
+        <v>200</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>121</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>240</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="4">
-        <v>400</v>
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>400</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>400</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>234</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="4"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>200</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>236</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="4"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>400</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>237</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="4"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="4">
+        <v>400</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>238</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="4"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="6">
+        <v>200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>241</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>400</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>242</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>400</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>243</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="4"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="5"/>
+      <c r="F13" s="1"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
+      <c r="F14" s="1"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
+      <c r="F15" s="1"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="4"/>
-      <c r="E17" s="1"/>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D18" s="4"/>
+      <c r="F18" s="1"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="4"/>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C19" s="4"/>
+      <c r="E19" s="1"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D20" s="4"/>
+      <c r="F20" s="1"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D21" s="4"/>
+      <c r="F21" s="1"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="4"/>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="1"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D23" s="4"/>
+      <c r="F23" s="1"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="1"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="1"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="5"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E34" s="5"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="5"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D162" s="4"/>
     </row>
-    <row r="163" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D163" s="4"/>
     </row>
-    <row r="164" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D164" s="4"/>
     </row>
-    <row r="165" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D165" s="4"/>
     </row>
-    <row r="166" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D166" s="4"/>
     </row>
-    <row r="167" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D168" s="4"/>
     </row>
-    <row r="169" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D169" s="4"/>
     </row>
-    <row r="170" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D170" s="4"/>
     </row>
-    <row r="171" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D171" s="4"/>
     </row>
-    <row r="172" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D172" s="4"/>
     </row>
-    <row r="173" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D173" s="4"/>
     </row>
-    <row r="174" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D174" s="4"/>
     </row>
-    <row r="175" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D176" s="4"/>
     </row>
-    <row r="177" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D183" s="4"/>
     </row>
-    <row r="184" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D184" s="4"/>
     </row>
-    <row r="185" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D187" s="4"/>
     </row>
-    <row r="188" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D188" s="4"/>
     </row>
-    <row r="189" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D190" s="4"/>
     </row>
-    <row r="191" spans="1:11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D191" s="4"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D192" s="4"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{D87B51C5-D291-4CA8-85C5-B9DA3EE47FFB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>